<commit_message>
Design basis sheets refactored
</commit_message>
<xml_diff>
--- a/thermax_backend/templates/enviro_ipg_design_basis_template.xlsx
+++ b/thermax_backend/templates/enviro_ipg_design_basis_template.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\abhishekraje30\frappe-bench\apps\thermax_backend\thermax_backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8931BF-6C5E-4D68-9FA0-64AA8CB3A1CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5734CE36-14F5-4E09-B621-36A964C547FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="COVER" sheetId="1" r:id="rId1"/>
     <sheet name="Design Basis" sheetId="2" r:id="rId2"/>
-    <sheet name="MCC" sheetId="3" r:id="rId3"/>
-    <sheet name="PCC" sheetId="6" r:id="rId4"/>
-    <sheet name="MCC CUM PLC" sheetId="5" r:id="rId5"/>
+    <sheet name="MCC VTUS88BP" sheetId="3" r:id="rId3"/>
+    <sheet name="PCC VTUS88BP" sheetId="6" r:id="rId4"/>
+    <sheet name="MCC CUM PLC VTUS88BP" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -1960,6 +1960,42 @@
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2011,41 +2047,77 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2059,6 +2131,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2077,81 +2152,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="14" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="21" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2185,12 +2185,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2199,21 +2214,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2709,7 +2709,7 @@
   </sheetPr>
   <dimension ref="A1:CD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView view="pageBreakPreview" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -3358,50 +3358,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="116.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="77"/>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="79"/>
+      <c r="A1" s="89"/>
+      <c r="B1" s="90"/>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="90"/>
+      <c r="F1" s="90"/>
+      <c r="G1" s="90"/>
+      <c r="H1" s="91"/>
     </row>
     <row r="2" spans="1:8" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="92" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="82"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="94"/>
     </row>
     <row r="3" spans="1:8" ht="23.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="83" t="s">
+      <c r="A3" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="85"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="97"/>
     </row>
     <row r="4" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="86" t="s">
+      <c r="A4" s="98" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="87"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="88"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="100"/>
     </row>
     <row r="5" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="29"/>
@@ -3415,78 +3415,78 @@
     </row>
     <row r="6" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="29"/>
-      <c r="B6" s="89" t="s">
+      <c r="B6" s="101" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="90"/>
-      <c r="D6" s="91" t="s">
+      <c r="C6" s="102"/>
+      <c r="D6" s="103" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="93"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="104"/>
+      <c r="G6" s="105"/>
       <c r="H6" s="30"/>
     </row>
     <row r="7" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="29"/>
-      <c r="B7" s="104" t="s">
+      <c r="B7" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="105"/>
-      <c r="D7" s="96"/>
-      <c r="E7" s="97"/>
-      <c r="F7" s="97"/>
-      <c r="G7" s="98"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="80"/>
+      <c r="F7" s="80"/>
+      <c r="G7" s="81"/>
       <c r="H7" s="30"/>
     </row>
     <row r="8" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="29"/>
-      <c r="B8" s="94" t="s">
+      <c r="B8" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="95"/>
-      <c r="D8" s="96"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="97"/>
-      <c r="G8" s="98"/>
+      <c r="C8" s="78"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="80"/>
+      <c r="F8" s="80"/>
+      <c r="G8" s="81"/>
       <c r="H8" s="30"/>
     </row>
     <row r="9" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="29"/>
-      <c r="B9" s="94" t="s">
+      <c r="B9" s="77" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="95"/>
-      <c r="D9" s="96"/>
-      <c r="E9" s="97"/>
-      <c r="F9" s="97"/>
-      <c r="G9" s="98"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="81"/>
       <c r="H9" s="30"/>
     </row>
     <row r="10" spans="1:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="29"/>
-      <c r="B10" s="94" t="s">
+      <c r="B10" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="95"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="97"/>
-      <c r="F10" s="97"/>
-      <c r="G10" s="98"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="81"/>
       <c r="H10" s="30"/>
     </row>
     <row r="11" spans="1:8" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="29"/>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="100"/>
-      <c r="D11" s="101" t="s">
+      <c r="C11" s="83"/>
+      <c r="D11" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="103"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="86"/>
       <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:8" s="31" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -3750,6 +3750,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G6"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:G10"/>
     <mergeCell ref="B11:C11"/>
@@ -3760,12 +3766,6 @@
     <mergeCell ref="D8:G8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:G9"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:G6"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="74" fitToHeight="100" orientation="portrait" r:id="rId1"/>
@@ -3791,26 +3791,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" s="110" t="s">
+      <c r="A1" s="135" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="111"/>
-      <c r="C1" s="111"/>
-      <c r="D1" s="112"/>
+      <c r="B1" s="136"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="137"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="113"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
-      <c r="D2" s="115"/>
+      <c r="A2" s="138"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="140"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
-      <c r="B3" s="116" t="s">
+      <c r="B3" s="108" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="117"/>
-      <c r="D3" s="118"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="110"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
@@ -3819,8 +3819,8 @@
       <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="108"/>
-      <c r="D4" s="109"/>
+      <c r="C4" s="132"/>
+      <c r="D4" s="133"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
@@ -3829,8 +3829,8 @@
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="108"/>
-      <c r="D5" s="109"/>
+      <c r="C5" s="132"/>
+      <c r="D5" s="133"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
@@ -3839,8 +3839,8 @@
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="109"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="133"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
@@ -3849,8 +3849,8 @@
       <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="108"/>
-      <c r="D7" s="109"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="133"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
@@ -3859,8 +3859,8 @@
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="106"/>
-      <c r="D8" s="107"/>
+      <c r="C8" s="130"/>
+      <c r="D8" s="131"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
@@ -3869,8 +3869,8 @@
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="108"/>
-      <c r="D9" s="109"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="133"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
@@ -3879,8 +3879,8 @@
       <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="106"/>
-      <c r="D10" s="107"/>
+      <c r="C10" s="130"/>
+      <c r="D10" s="131"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
@@ -3889,8 +3889,8 @@
       <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="106"/>
-      <c r="D11" s="107"/>
+      <c r="C11" s="130"/>
+      <c r="D11" s="131"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
@@ -3899,8 +3899,8 @@
       <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="106"/>
-      <c r="D12" s="107"/>
+      <c r="C12" s="130"/>
+      <c r="D12" s="131"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
@@ -3909,8 +3909,8 @@
       <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="106"/>
-      <c r="D13" s="107"/>
+      <c r="C13" s="130"/>
+      <c r="D13" s="131"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
@@ -3919,8 +3919,8 @@
       <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="119"/>
-      <c r="D14" s="107"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="131"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
@@ -3929,8 +3929,8 @@
       <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="119"/>
-      <c r="D15" s="107"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="131"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
@@ -3939,8 +3939,8 @@
       <c r="B16" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="119"/>
-      <c r="D16" s="107"/>
+      <c r="C16" s="134"/>
+      <c r="D16" s="131"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
@@ -3949,8 +3949,8 @@
       <c r="B17" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="119"/>
-      <c r="D17" s="107"/>
+      <c r="C17" s="134"/>
+      <c r="D17" s="131"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
@@ -3959,16 +3959,16 @@
       <c r="B18" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="106"/>
-      <c r="D18" s="107"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="131"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
-      <c r="B19" s="116" t="s">
+      <c r="B19" s="108" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="117"/>
-      <c r="D19" s="118"/>
+      <c r="C19" s="109"/>
+      <c r="D19" s="110"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
@@ -3977,8 +3977,8 @@
       <c r="B20" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="106"/>
-      <c r="D20" s="107"/>
+      <c r="C20" s="130"/>
+      <c r="D20" s="131"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
@@ -3987,8 +3987,8 @@
       <c r="B21" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="108"/>
-      <c r="D21" s="109"/>
+      <c r="C21" s="132"/>
+      <c r="D21" s="133"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
@@ -3997,8 +3997,8 @@
       <c r="B22" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="106"/>
-      <c r="D22" s="107"/>
+      <c r="C22" s="130"/>
+      <c r="D22" s="131"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
@@ -4007,8 +4007,8 @@
       <c r="B23" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C23" s="106"/>
-      <c r="D23" s="107"/>
+      <c r="C23" s="130"/>
+      <c r="D23" s="131"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
@@ -4017,16 +4017,16 @@
       <c r="B24" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="C24" s="108"/>
-      <c r="D24" s="109"/>
+      <c r="C24" s="132"/>
+      <c r="D24" s="133"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
-      <c r="B25" s="116" t="s">
+      <c r="B25" s="108" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="117"/>
-      <c r="D25" s="118"/>
+      <c r="C25" s="109"/>
+      <c r="D25" s="110"/>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="27"/>
@@ -4252,19 +4252,19 @@
     </row>
     <row r="48" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
-      <c r="B48" s="116" t="s">
+      <c r="B48" s="108" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="117"/>
-      <c r="D48" s="118"/>
+      <c r="C48" s="109"/>
+      <c r="D48" s="110"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
-      <c r="B49" s="116" t="s">
+      <c r="B49" s="108" t="s">
         <v>65</v>
       </c>
-      <c r="C49" s="117"/>
-      <c r="D49" s="118"/>
+      <c r="C49" s="109"/>
+      <c r="D49" s="110"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
@@ -4273,8 +4273,8 @@
       <c r="B50" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="C50" s="120"/>
-      <c r="D50" s="121"/>
+      <c r="C50" s="106"/>
+      <c r="D50" s="107"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
@@ -4283,8 +4283,8 @@
       <c r="B51" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="C51" s="120"/>
-      <c r="D51" s="121"/>
+      <c r="C51" s="106"/>
+      <c r="D51" s="107"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
@@ -4293,8 +4293,8 @@
       <c r="B52" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="C52" s="120"/>
-      <c r="D52" s="121"/>
+      <c r="C52" s="106"/>
+      <c r="D52" s="107"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
@@ -4303,8 +4303,8 @@
       <c r="B53" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="C53" s="120"/>
-      <c r="D53" s="121"/>
+      <c r="C53" s="106"/>
+      <c r="D53" s="107"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
@@ -4313,8 +4313,8 @@
       <c r="B54" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="C54" s="120"/>
-      <c r="D54" s="121"/>
+      <c r="C54" s="106"/>
+      <c r="D54" s="107"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
@@ -4323,8 +4323,8 @@
       <c r="B55" s="62" t="s">
         <v>71</v>
       </c>
-      <c r="C55" s="120"/>
-      <c r="D55" s="121"/>
+      <c r="C55" s="106"/>
+      <c r="D55" s="107"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
@@ -4333,24 +4333,24 @@
       <c r="B56" s="62" t="s">
         <v>72</v>
       </c>
-      <c r="C56" s="120"/>
-      <c r="D56" s="121"/>
+      <c r="C56" s="106"/>
+      <c r="D56" s="107"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
-      <c r="B57" s="116" t="s">
+      <c r="B57" s="108" t="s">
         <v>73</v>
       </c>
-      <c r="C57" s="117"/>
-      <c r="D57" s="118"/>
+      <c r="C57" s="109"/>
+      <c r="D57" s="110"/>
     </row>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
-      <c r="B58" s="116" t="s">
+      <c r="B58" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="C58" s="117"/>
-      <c r="D58" s="118"/>
+      <c r="C58" s="109"/>
+      <c r="D58" s="110"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
@@ -4359,16 +4359,16 @@
       <c r="B59" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="120"/>
-      <c r="D59" s="121"/>
+      <c r="C59" s="106"/>
+      <c r="D59" s="107"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
-      <c r="B60" s="116" t="s">
+      <c r="B60" s="108" t="s">
         <v>76</v>
       </c>
-      <c r="C60" s="117"/>
-      <c r="D60" s="118"/>
+      <c r="C60" s="109"/>
+      <c r="D60" s="110"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
@@ -4377,8 +4377,8 @@
       <c r="B61" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C61" s="122"/>
-      <c r="D61" s="123"/>
+      <c r="C61" s="116"/>
+      <c r="D61" s="112"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
@@ -4387,8 +4387,8 @@
       <c r="B62" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C62" s="122"/>
-      <c r="D62" s="123"/>
+      <c r="C62" s="116"/>
+      <c r="D62" s="112"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
@@ -4397,8 +4397,8 @@
       <c r="B63" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C63" s="122"/>
-      <c r="D63" s="123"/>
+      <c r="C63" s="116"/>
+      <c r="D63" s="112"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
@@ -4407,8 +4407,8 @@
       <c r="B64" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C64" s="122"/>
-      <c r="D64" s="123"/>
+      <c r="C64" s="116"/>
+      <c r="D64" s="112"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
@@ -4417,8 +4417,8 @@
       <c r="B65" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C65" s="122"/>
-      <c r="D65" s="123"/>
+      <c r="C65" s="116"/>
+      <c r="D65" s="112"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
@@ -4427,16 +4427,16 @@
       <c r="B66" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C66" s="122"/>
-      <c r="D66" s="123"/>
+      <c r="C66" s="116"/>
+      <c r="D66" s="112"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
-      <c r="B67" s="116" t="s">
+      <c r="B67" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="C67" s="117"/>
-      <c r="D67" s="118"/>
+      <c r="C67" s="109"/>
+      <c r="D67" s="110"/>
     </row>
     <row r="68" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="12">
@@ -4445,16 +4445,16 @@
       <c r="B68" s="64" t="s">
         <v>84</v>
       </c>
-      <c r="C68" s="120"/>
-      <c r="D68" s="121"/>
+      <c r="C68" s="106"/>
+      <c r="D68" s="107"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
-      <c r="B69" s="116" t="s">
+      <c r="B69" s="108" t="s">
         <v>85</v>
       </c>
-      <c r="C69" s="117"/>
-      <c r="D69" s="118"/>
+      <c r="C69" s="109"/>
+      <c r="D69" s="110"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
@@ -4463,8 +4463,8 @@
       <c r="B70" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="C70" s="120"/>
-      <c r="D70" s="121"/>
+      <c r="C70" s="106"/>
+      <c r="D70" s="107"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
@@ -4473,8 +4473,8 @@
       <c r="B71" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="C71" s="120"/>
-      <c r="D71" s="121"/>
+      <c r="C71" s="106"/>
+      <c r="D71" s="107"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
@@ -4483,8 +4483,8 @@
       <c r="B72" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="C72" s="120"/>
-      <c r="D72" s="121"/>
+      <c r="C72" s="106"/>
+      <c r="D72" s="107"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
@@ -4493,8 +4493,8 @@
       <c r="B73" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="C73" s="120"/>
-      <c r="D73" s="121"/>
+      <c r="C73" s="106"/>
+      <c r="D73" s="107"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
@@ -4503,16 +4503,16 @@
       <c r="B74" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="C74" s="120"/>
-      <c r="D74" s="121"/>
+      <c r="C74" s="106"/>
+      <c r="D74" s="107"/>
     </row>
     <row r="75" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
-      <c r="B75" s="124" t="s">
+      <c r="B75" s="128" t="s">
         <v>91</v>
       </c>
-      <c r="C75" s="124"/>
-      <c r="D75" s="125"/>
+      <c r="C75" s="128"/>
+      <c r="D75" s="129"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
@@ -4521,8 +4521,8 @@
       <c r="B76" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="C76" s="120"/>
-      <c r="D76" s="121"/>
+      <c r="C76" s="106"/>
+      <c r="D76" s="107"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
@@ -4531,8 +4531,8 @@
       <c r="B77" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="C77" s="120"/>
-      <c r="D77" s="121"/>
+      <c r="C77" s="106"/>
+      <c r="D77" s="107"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
@@ -4541,8 +4541,8 @@
       <c r="B78" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="C78" s="120"/>
-      <c r="D78" s="121"/>
+      <c r="C78" s="106"/>
+      <c r="D78" s="107"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
@@ -4551,8 +4551,8 @@
       <c r="B79" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="C79" s="120"/>
-      <c r="D79" s="121"/>
+      <c r="C79" s="106"/>
+      <c r="D79" s="107"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
@@ -4561,16 +4561,16 @@
       <c r="B80" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="C80" s="120"/>
-      <c r="D80" s="121"/>
+      <c r="C80" s="106"/>
+      <c r="D80" s="107"/>
     </row>
     <row r="81" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
-      <c r="B81" s="124" t="s">
+      <c r="B81" s="128" t="s">
         <v>93</v>
       </c>
-      <c r="C81" s="124"/>
-      <c r="D81" s="125"/>
+      <c r="C81" s="128"/>
+      <c r="D81" s="129"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
@@ -4579,8 +4579,8 @@
       <c r="B82" s="62" t="s">
         <v>86</v>
       </c>
-      <c r="C82" s="120"/>
-      <c r="D82" s="121"/>
+      <c r="C82" s="106"/>
+      <c r="D82" s="107"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
@@ -4589,8 +4589,8 @@
       <c r="B83" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="C83" s="120"/>
-      <c r="D83" s="121"/>
+      <c r="C83" s="106"/>
+      <c r="D83" s="107"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
@@ -4599,8 +4599,8 @@
       <c r="B84" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="C84" s="120"/>
-      <c r="D84" s="121"/>
+      <c r="C84" s="106"/>
+      <c r="D84" s="107"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
@@ -4609,8 +4609,8 @@
       <c r="B85" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="C85" s="120"/>
-      <c r="D85" s="121"/>
+      <c r="C85" s="106"/>
+      <c r="D85" s="107"/>
     </row>
     <row r="86" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
@@ -4619,8 +4619,8 @@
       <c r="B86" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="C86" s="120"/>
-      <c r="D86" s="121"/>
+      <c r="C86" s="106"/>
+      <c r="D86" s="107"/>
     </row>
     <row r="87" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
@@ -4629,8 +4629,8 @@
       <c r="B87" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C87" s="120"/>
-      <c r="D87" s="121"/>
+      <c r="C87" s="106"/>
+      <c r="D87" s="107"/>
     </row>
     <row r="88" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
@@ -4639,8 +4639,8 @@
       <c r="B88" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="C88" s="120"/>
-      <c r="D88" s="121"/>
+      <c r="C88" s="106"/>
+      <c r="D88" s="107"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
@@ -4649,16 +4649,16 @@
       <c r="B89" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="C89" s="120"/>
-      <c r="D89" s="121"/>
+      <c r="C89" s="106"/>
+      <c r="D89" s="107"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90" s="1"/>
-      <c r="B90" s="116" t="s">
+      <c r="B90" s="108" t="s">
         <v>98</v>
       </c>
-      <c r="C90" s="117"/>
-      <c r="D90" s="118"/>
+      <c r="C90" s="109"/>
+      <c r="D90" s="110"/>
     </row>
     <row r="91" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
@@ -4667,8 +4667,8 @@
       <c r="B91" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="C91" s="120"/>
-      <c r="D91" s="121"/>
+      <c r="C91" s="106"/>
+      <c r="D91" s="107"/>
     </row>
     <row r="92" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
@@ -4677,8 +4677,8 @@
       <c r="B92" s="62" t="s">
         <v>100</v>
       </c>
-      <c r="C92" s="120"/>
-      <c r="D92" s="121"/>
+      <c r="C92" s="106"/>
+      <c r="D92" s="107"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
@@ -4687,8 +4687,8 @@
       <c r="B93" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="C93" s="120"/>
-      <c r="D93" s="121"/>
+      <c r="C93" s="106"/>
+      <c r="D93" s="107"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
@@ -4697,16 +4697,16 @@
       <c r="B94" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="C94" s="120"/>
-      <c r="D94" s="121"/>
+      <c r="C94" s="106"/>
+      <c r="D94" s="107"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95" s="1"/>
-      <c r="B95" s="116" t="s">
+      <c r="B95" s="108" t="s">
         <v>103</v>
       </c>
-      <c r="C95" s="117"/>
-      <c r="D95" s="118"/>
+      <c r="C95" s="109"/>
+      <c r="D95" s="110"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
@@ -4715,8 +4715,8 @@
       <c r="B96" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="C96" s="120"/>
-      <c r="D96" s="121"/>
+      <c r="C96" s="106"/>
+      <c r="D96" s="107"/>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
@@ -4725,8 +4725,8 @@
       <c r="B97" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="C97" s="122"/>
-      <c r="D97" s="123"/>
+      <c r="C97" s="116"/>
+      <c r="D97" s="112"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
@@ -4735,8 +4735,8 @@
       <c r="B98" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C98" s="120"/>
-      <c r="D98" s="121"/>
+      <c r="C98" s="106"/>
+      <c r="D98" s="107"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
@@ -4745,8 +4745,8 @@
       <c r="B99" s="62" t="s">
         <v>107</v>
       </c>
-      <c r="C99" s="120"/>
-      <c r="D99" s="121"/>
+      <c r="C99" s="106"/>
+      <c r="D99" s="107"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
@@ -4755,16 +4755,16 @@
       <c r="B100" s="62" t="s">
         <v>108</v>
       </c>
-      <c r="C100" s="120"/>
-      <c r="D100" s="121"/>
+      <c r="C100" s="106"/>
+      <c r="D100" s="107"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101" s="1"/>
-      <c r="B101" s="116" t="s">
+      <c r="B101" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="C101" s="117"/>
-      <c r="D101" s="118"/>
+      <c r="C101" s="109"/>
+      <c r="D101" s="110"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
@@ -4773,8 +4773,8 @@
       <c r="B102" s="62" t="s">
         <v>110</v>
       </c>
-      <c r="C102" s="122"/>
-      <c r="D102" s="123"/>
+      <c r="C102" s="116"/>
+      <c r="D102" s="112"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
@@ -4783,8 +4783,8 @@
       <c r="B103" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="C103" s="122"/>
-      <c r="D103" s="123"/>
+      <c r="C103" s="116"/>
+      <c r="D103" s="112"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
@@ -4793,8 +4793,8 @@
       <c r="B104" s="62" t="s">
         <v>112</v>
       </c>
-      <c r="C104" s="122"/>
-      <c r="D104" s="123"/>
+      <c r="C104" s="116"/>
+      <c r="D104" s="112"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
@@ -4803,16 +4803,16 @@
       <c r="B105" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="C105" s="122"/>
-      <c r="D105" s="123"/>
+      <c r="C105" s="116"/>
+      <c r="D105" s="112"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" s="1"/>
-      <c r="B106" s="116" t="s">
+      <c r="B106" s="108" t="s">
         <v>114</v>
       </c>
-      <c r="C106" s="117"/>
-      <c r="D106" s="118"/>
+      <c r="C106" s="109"/>
+      <c r="D106" s="110"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
@@ -4821,16 +4821,16 @@
       <c r="B107" s="64" t="s">
         <v>115</v>
       </c>
-      <c r="C107" s="120"/>
-      <c r="D107" s="121"/>
+      <c r="C107" s="106"/>
+      <c r="D107" s="107"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" s="1"/>
-      <c r="B108" s="116" t="s">
+      <c r="B108" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="C108" s="117"/>
-      <c r="D108" s="118"/>
+      <c r="C108" s="109"/>
+      <c r="D108" s="110"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
@@ -4839,8 +4839,8 @@
       <c r="B109" s="62" t="s">
         <v>117</v>
       </c>
-      <c r="C109" s="120"/>
-      <c r="D109" s="121"/>
+      <c r="C109" s="106"/>
+      <c r="D109" s="107"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
@@ -4849,8 +4849,8 @@
       <c r="B110" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="C110" s="120"/>
-      <c r="D110" s="121"/>
+      <c r="C110" s="106"/>
+      <c r="D110" s="107"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
@@ -4859,8 +4859,8 @@
       <c r="B111" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="C111" s="120"/>
-      <c r="D111" s="121"/>
+      <c r="C111" s="106"/>
+      <c r="D111" s="107"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
@@ -4869,8 +4869,8 @@
       <c r="B112" s="62" t="s">
         <v>120</v>
       </c>
-      <c r="C112" s="120"/>
-      <c r="D112" s="121"/>
+      <c r="C112" s="106"/>
+      <c r="D112" s="107"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
@@ -4879,8 +4879,8 @@
       <c r="B113" s="62" t="s">
         <v>121</v>
       </c>
-      <c r="C113" s="120"/>
-      <c r="D113" s="121"/>
+      <c r="C113" s="106"/>
+      <c r="D113" s="107"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
@@ -4889,8 +4889,8 @@
       <c r="B114" s="62" t="s">
         <v>122</v>
       </c>
-      <c r="C114" s="120"/>
-      <c r="D114" s="121"/>
+      <c r="C114" s="106"/>
+      <c r="D114" s="107"/>
     </row>
     <row r="115" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
@@ -4899,8 +4899,8 @@
       <c r="B115" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="C115" s="120"/>
-      <c r="D115" s="121"/>
+      <c r="C115" s="106"/>
+      <c r="D115" s="107"/>
     </row>
     <row r="116" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
@@ -4909,8 +4909,8 @@
       <c r="B116" s="62" t="s">
         <v>124</v>
       </c>
-      <c r="C116" s="120"/>
-      <c r="D116" s="121"/>
+      <c r="C116" s="106"/>
+      <c r="D116" s="107"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
@@ -4919,8 +4919,8 @@
       <c r="B117" s="62" t="s">
         <v>125</v>
       </c>
-      <c r="C117" s="120"/>
-      <c r="D117" s="121"/>
+      <c r="C117" s="106"/>
+      <c r="D117" s="107"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
@@ -4929,8 +4929,8 @@
       <c r="B118" s="62" t="s">
         <v>126</v>
       </c>
-      <c r="C118" s="120"/>
-      <c r="D118" s="121"/>
+      <c r="C118" s="106"/>
+      <c r="D118" s="107"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
@@ -4939,8 +4939,8 @@
       <c r="B119" s="62" t="s">
         <v>127</v>
       </c>
-      <c r="C119" s="122"/>
-      <c r="D119" s="123"/>
+      <c r="C119" s="116"/>
+      <c r="D119" s="112"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
@@ -4949,8 +4949,8 @@
       <c r="B120" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="C120" s="122"/>
-      <c r="D120" s="123"/>
+      <c r="C120" s="116"/>
+      <c r="D120" s="112"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
@@ -4959,8 +4959,8 @@
       <c r="B121" s="62" t="s">
         <v>129</v>
       </c>
-      <c r="C121" s="122"/>
-      <c r="D121" s="123"/>
+      <c r="C121" s="116"/>
+      <c r="D121" s="112"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
@@ -4969,8 +4969,8 @@
       <c r="B122" s="62" t="s">
         <v>130</v>
       </c>
-      <c r="C122" s="122"/>
-      <c r="D122" s="123"/>
+      <c r="C122" s="116"/>
+      <c r="D122" s="112"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
@@ -4979,8 +4979,8 @@
       <c r="B123" s="62" t="s">
         <v>131</v>
       </c>
-      <c r="C123" s="120"/>
-      <c r="D123" s="121"/>
+      <c r="C123" s="106"/>
+      <c r="D123" s="107"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
@@ -4989,8 +4989,8 @@
       <c r="B124" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="C124" s="120"/>
-      <c r="D124" s="121"/>
+      <c r="C124" s="106"/>
+      <c r="D124" s="107"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
@@ -4999,12 +4999,12 @@
       <c r="B125" s="62" t="s">
         <v>133</v>
       </c>
-      <c r="C125" s="120"/>
-      <c r="D125" s="121"/>
+      <c r="C125" s="106"/>
+      <c r="D125" s="107"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126" s="9"/>
-      <c r="B126" s="116" t="s">
+      <c r="B126" s="108" t="s">
         <v>134</v>
       </c>
       <c r="C126" s="126"/>
@@ -5017,8 +5017,8 @@
       <c r="B127" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C127" s="120"/>
-      <c r="D127" s="121"/>
+      <c r="C127" s="106"/>
+      <c r="D127" s="107"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128" s="9">
@@ -5027,8 +5027,8 @@
       <c r="B128" s="62" t="s">
         <v>136</v>
       </c>
-      <c r="C128" s="120"/>
-      <c r="D128" s="121"/>
+      <c r="C128" s="106"/>
+      <c r="D128" s="107"/>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129" s="9">
@@ -5037,8 +5037,8 @@
       <c r="B129" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C129" s="120"/>
-      <c r="D129" s="121"/>
+      <c r="C129" s="106"/>
+      <c r="D129" s="107"/>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130" s="9">
@@ -5047,16 +5047,16 @@
       <c r="B130" s="62" t="s">
         <v>138</v>
       </c>
-      <c r="C130" s="122"/>
-      <c r="D130" s="123"/>
+      <c r="C130" s="116"/>
+      <c r="D130" s="112"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131" s="1"/>
-      <c r="B131" s="116" t="s">
+      <c r="B131" s="108" t="s">
         <v>139</v>
       </c>
-      <c r="C131" s="117"/>
-      <c r="D131" s="118"/>
+      <c r="C131" s="109"/>
+      <c r="D131" s="110"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
@@ -5065,8 +5065,8 @@
       <c r="B132" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="C132" s="120"/>
-      <c r="D132" s="121"/>
+      <c r="C132" s="106"/>
+      <c r="D132" s="107"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
@@ -5075,8 +5075,8 @@
       <c r="B133" s="57" t="s">
         <v>141</v>
       </c>
-      <c r="C133" s="120"/>
-      <c r="D133" s="121"/>
+      <c r="C133" s="106"/>
+      <c r="D133" s="107"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
@@ -5085,8 +5085,8 @@
       <c r="B134" s="57" t="s">
         <v>142</v>
       </c>
-      <c r="C134" s="122"/>
-      <c r="D134" s="123"/>
+      <c r="C134" s="116"/>
+      <c r="D134" s="112"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
@@ -5095,8 +5095,8 @@
       <c r="B135" s="57" t="s">
         <v>143</v>
       </c>
-      <c r="C135" s="120"/>
-      <c r="D135" s="121"/>
+      <c r="C135" s="106"/>
+      <c r="D135" s="107"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
@@ -5105,8 +5105,8 @@
       <c r="B136" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="C136" s="120"/>
-      <c r="D136" s="121"/>
+      <c r="C136" s="106"/>
+      <c r="D136" s="107"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
@@ -5115,8 +5115,8 @@
       <c r="B137" s="57" t="s">
         <v>145</v>
       </c>
-      <c r="C137" s="122"/>
-      <c r="D137" s="123"/>
+      <c r="C137" s="116"/>
+      <c r="D137" s="112"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
@@ -5125,8 +5125,8 @@
       <c r="B138" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="C138" s="120"/>
-      <c r="D138" s="121"/>
+      <c r="C138" s="106"/>
+      <c r="D138" s="107"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
@@ -5135,8 +5135,8 @@
       <c r="B139" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="C139" s="120"/>
-      <c r="D139" s="121"/>
+      <c r="C139" s="106"/>
+      <c r="D139" s="107"/>
     </row>
     <row r="140" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
@@ -5145,8 +5145,8 @@
       <c r="B140" s="57" t="s">
         <v>148</v>
       </c>
-      <c r="C140" s="122"/>
-      <c r="D140" s="123"/>
+      <c r="C140" s="116"/>
+      <c r="D140" s="112"/>
     </row>
     <row r="141" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
@@ -5155,8 +5155,8 @@
       <c r="B141" s="57" t="s">
         <v>149</v>
       </c>
-      <c r="C141" s="122"/>
-      <c r="D141" s="123"/>
+      <c r="C141" s="116"/>
+      <c r="D141" s="112"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
@@ -5165,8 +5165,8 @@
       <c r="B142" s="57" t="s">
         <v>150</v>
       </c>
-      <c r="C142" s="120"/>
-      <c r="D142" s="121"/>
+      <c r="C142" s="106"/>
+      <c r="D142" s="107"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
@@ -5175,16 +5175,16 @@
       <c r="B143" s="57" t="s">
         <v>151</v>
       </c>
-      <c r="C143" s="137"/>
-      <c r="D143" s="123"/>
+      <c r="C143" s="111"/>
+      <c r="D143" s="112"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144" s="1"/>
-      <c r="B144" s="116" t="s">
+      <c r="B144" s="108" t="s">
         <v>152</v>
       </c>
-      <c r="C144" s="117"/>
-      <c r="D144" s="118"/>
+      <c r="C144" s="109"/>
+      <c r="D144" s="110"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
@@ -5193,16 +5193,16 @@
       <c r="B145" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C145" s="130"/>
-      <c r="D145" s="131"/>
+      <c r="C145" s="124"/>
+      <c r="D145" s="125"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146" s="1"/>
-      <c r="B146" s="116" t="s">
+      <c r="B146" s="108" t="s">
         <v>154</v>
       </c>
-      <c r="C146" s="117"/>
-      <c r="D146" s="118"/>
+      <c r="C146" s="109"/>
+      <c r="D146" s="110"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
@@ -5211,8 +5211,8 @@
       <c r="B147" s="62" t="s">
         <v>155</v>
       </c>
-      <c r="C147" s="120"/>
-      <c r="D147" s="121"/>
+      <c r="C147" s="106"/>
+      <c r="D147" s="107"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
@@ -5221,8 +5221,8 @@
       <c r="B148" s="62" t="s">
         <v>156</v>
       </c>
-      <c r="C148" s="120"/>
-      <c r="D148" s="121"/>
+      <c r="C148" s="106"/>
+      <c r="D148" s="107"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
@@ -5231,16 +5231,16 @@
       <c r="B149" s="62" t="s">
         <v>157</v>
       </c>
-      <c r="C149" s="120"/>
-      <c r="D149" s="121"/>
+      <c r="C149" s="106"/>
+      <c r="D149" s="107"/>
     </row>
     <row r="150" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" s="1"/>
-      <c r="B150" s="116" t="s">
+      <c r="B150" s="108" t="s">
         <v>158</v>
       </c>
-      <c r="C150" s="117"/>
-      <c r="D150" s="118"/>
+      <c r="C150" s="109"/>
+      <c r="D150" s="110"/>
     </row>
     <row r="151" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="1"/>
@@ -5326,11 +5326,11 @@
     </row>
     <row r="159" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="1"/>
-      <c r="B159" s="116" t="s">
+      <c r="B159" s="108" t="s">
         <v>167</v>
       </c>
-      <c r="C159" s="117"/>
-      <c r="D159" s="118"/>
+      <c r="C159" s="109"/>
+      <c r="D159" s="110"/>
     </row>
     <row r="160" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
@@ -5339,8 +5339,8 @@
       <c r="B160" s="62" t="s">
         <v>140</v>
       </c>
-      <c r="C160" s="128"/>
-      <c r="D160" s="129"/>
+      <c r="C160" s="117"/>
+      <c r="D160" s="118"/>
     </row>
     <row r="161" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
@@ -5349,8 +5349,8 @@
       <c r="B161" s="62" t="s">
         <v>143</v>
       </c>
-      <c r="C161" s="128"/>
-      <c r="D161" s="129"/>
+      <c r="C161" s="117"/>
+      <c r="D161" s="118"/>
     </row>
     <row r="162" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
@@ -5359,8 +5359,8 @@
       <c r="B162" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="C162" s="128"/>
-      <c r="D162" s="129"/>
+      <c r="C162" s="117"/>
+      <c r="D162" s="118"/>
     </row>
     <row r="163" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
@@ -5369,8 +5369,8 @@
       <c r="B163" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="C163" s="128"/>
-      <c r="D163" s="129"/>
+      <c r="C163" s="117"/>
+      <c r="D163" s="118"/>
     </row>
     <row r="164" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
@@ -5379,8 +5379,8 @@
       <c r="B164" s="62" t="s">
         <v>146</v>
       </c>
-      <c r="C164" s="128"/>
-      <c r="D164" s="129"/>
+      <c r="C164" s="117"/>
+      <c r="D164" s="118"/>
     </row>
     <row r="165" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
@@ -5389,8 +5389,8 @@
       <c r="B165" s="62" t="s">
         <v>147</v>
       </c>
-      <c r="C165" s="128"/>
-      <c r="D165" s="129"/>
+      <c r="C165" s="117"/>
+      <c r="D165" s="118"/>
     </row>
     <row r="166" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
@@ -5399,8 +5399,8 @@
       <c r="B166" s="62" t="s">
         <v>169</v>
       </c>
-      <c r="C166" s="128"/>
-      <c r="D166" s="129"/>
+      <c r="C166" s="117"/>
+      <c r="D166" s="118"/>
     </row>
     <row r="167" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
@@ -5409,8 +5409,8 @@
       <c r="B167" s="62" t="s">
         <v>170</v>
       </c>
-      <c r="C167" s="128"/>
-      <c r="D167" s="129"/>
+      <c r="C167" s="117"/>
+      <c r="D167" s="118"/>
     </row>
     <row r="168" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="1"/>
@@ -5496,11 +5496,11 @@
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176" s="1"/>
-      <c r="B176" s="116" t="s">
+      <c r="B176" s="108" t="s">
         <v>172</v>
       </c>
-      <c r="C176" s="117"/>
-      <c r="D176" s="118"/>
+      <c r="C176" s="109"/>
+      <c r="D176" s="110"/>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
@@ -5509,8 +5509,8 @@
       <c r="B177" s="62" t="s">
         <v>173</v>
       </c>
-      <c r="C177" s="120"/>
-      <c r="D177" s="121"/>
+      <c r="C177" s="106"/>
+      <c r="D177" s="107"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
@@ -5519,8 +5519,8 @@
       <c r="B178" s="62" t="s">
         <v>174</v>
       </c>
-      <c r="C178" s="120"/>
-      <c r="D178" s="121"/>
+      <c r="C178" s="106"/>
+      <c r="D178" s="107"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
@@ -5529,16 +5529,16 @@
       <c r="B179" s="62" t="s">
         <v>175</v>
       </c>
-      <c r="C179" s="122"/>
-      <c r="D179" s="123"/>
+      <c r="C179" s="116"/>
+      <c r="D179" s="112"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180" s="1"/>
-      <c r="B180" s="116" t="s">
+      <c r="B180" s="108" t="s">
         <v>176</v>
       </c>
-      <c r="C180" s="117"/>
-      <c r="D180" s="118"/>
+      <c r="C180" s="109"/>
+      <c r="D180" s="110"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
@@ -5547,8 +5547,8 @@
       <c r="B181" s="62" t="s">
         <v>177</v>
       </c>
-      <c r="C181" s="128"/>
-      <c r="D181" s="129"/>
+      <c r="C181" s="117"/>
+      <c r="D181" s="118"/>
     </row>
     <row r="182" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
@@ -5557,16 +5557,16 @@
       <c r="B182" s="62" t="s">
         <v>178</v>
       </c>
-      <c r="C182" s="120"/>
-      <c r="D182" s="121"/>
+      <c r="C182" s="106"/>
+      <c r="D182" s="107"/>
     </row>
     <row r="183" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="12"/>
-      <c r="B183" s="116" t="s">
+      <c r="B183" s="108" t="s">
         <v>179</v>
       </c>
-      <c r="C183" s="117"/>
-      <c r="D183" s="118"/>
+      <c r="C183" s="109"/>
+      <c r="D183" s="110"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
@@ -5575,8 +5575,8 @@
       <c r="B184" s="62" t="s">
         <v>180</v>
       </c>
-      <c r="C184" s="120"/>
-      <c r="D184" s="121"/>
+      <c r="C184" s="106"/>
+      <c r="D184" s="107"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
@@ -5585,8 +5585,8 @@
       <c r="B185" s="62" t="s">
         <v>181</v>
       </c>
-      <c r="C185" s="120"/>
-      <c r="D185" s="121"/>
+      <c r="C185" s="106"/>
+      <c r="D185" s="107"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
@@ -5595,8 +5595,8 @@
       <c r="B186" s="62" t="s">
         <v>182</v>
       </c>
-      <c r="C186" s="120"/>
-      <c r="D186" s="121"/>
+      <c r="C186" s="106"/>
+      <c r="D186" s="107"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
@@ -5605,8 +5605,8 @@
       <c r="B187" s="62" t="s">
         <v>183</v>
       </c>
-      <c r="C187" s="120"/>
-      <c r="D187" s="121"/>
+      <c r="C187" s="106"/>
+      <c r="D187" s="107"/>
     </row>
     <row r="188" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
@@ -5615,8 +5615,8 @@
       <c r="B188" s="62" t="s">
         <v>184</v>
       </c>
-      <c r="C188" s="138"/>
-      <c r="D188" s="139"/>
+      <c r="C188" s="113"/>
+      <c r="D188" s="114"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
@@ -5625,8 +5625,8 @@
       <c r="B189" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="C189" s="140"/>
-      <c r="D189" s="121"/>
+      <c r="C189" s="115"/>
+      <c r="D189" s="107"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
@@ -5635,8 +5635,8 @@
       <c r="B190" s="62" t="s">
         <v>186</v>
       </c>
-      <c r="C190" s="122"/>
-      <c r="D190" s="123"/>
+      <c r="C190" s="116"/>
+      <c r="D190" s="112"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
@@ -5645,8 +5645,8 @@
       <c r="B191" s="62" t="s">
         <v>187</v>
       </c>
-      <c r="C191" s="120"/>
-      <c r="D191" s="121"/>
+      <c r="C191" s="106"/>
+      <c r="D191" s="107"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
@@ -5655,8 +5655,8 @@
       <c r="B192" s="62" t="s">
         <v>188</v>
       </c>
-      <c r="C192" s="120"/>
-      <c r="D192" s="121"/>
+      <c r="C192" s="106"/>
+      <c r="D192" s="107"/>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
@@ -5665,8 +5665,8 @@
       <c r="B193" s="62" t="s">
         <v>189</v>
       </c>
-      <c r="C193" s="120"/>
-      <c r="D193" s="121"/>
+      <c r="C193" s="106"/>
+      <c r="D193" s="107"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
@@ -5675,8 +5675,8 @@
       <c r="B194" s="62" t="s">
         <v>190</v>
       </c>
-      <c r="C194" s="120"/>
-      <c r="D194" s="121"/>
+      <c r="C194" s="106"/>
+      <c r="D194" s="107"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
@@ -5685,8 +5685,8 @@
       <c r="B195" s="62" t="s">
         <v>191</v>
       </c>
-      <c r="C195" s="120"/>
-      <c r="D195" s="121"/>
+      <c r="C195" s="106"/>
+      <c r="D195" s="107"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
@@ -5695,8 +5695,8 @@
       <c r="B196" s="62" t="s">
         <v>192</v>
       </c>
-      <c r="C196" s="120"/>
-      <c r="D196" s="121"/>
+      <c r="C196" s="106"/>
+      <c r="D196" s="107"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
@@ -5705,8 +5705,8 @@
       <c r="B197" s="62" t="s">
         <v>193</v>
       </c>
-      <c r="C197" s="120"/>
-      <c r="D197" s="121"/>
+      <c r="C197" s="106"/>
+      <c r="D197" s="107"/>
     </row>
     <row r="198" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
@@ -5715,16 +5715,16 @@
       <c r="B198" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="C198" s="120"/>
-      <c r="D198" s="121"/>
+      <c r="C198" s="106"/>
+      <c r="D198" s="107"/>
     </row>
     <row r="199" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" s="1"/>
-      <c r="B199" s="116" t="s">
+      <c r="B199" s="108" t="s">
         <v>195</v>
       </c>
-      <c r="C199" s="117"/>
-      <c r="D199" s="118"/>
+      <c r="C199" s="109"/>
+      <c r="D199" s="110"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
@@ -5733,8 +5733,8 @@
       <c r="B200" s="62" t="s">
         <v>196</v>
       </c>
-      <c r="C200" s="120"/>
-      <c r="D200" s="121"/>
+      <c r="C200" s="106"/>
+      <c r="D200" s="107"/>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
@@ -5743,8 +5743,8 @@
       <c r="B201" s="62" t="s">
         <v>197</v>
       </c>
-      <c r="C201" s="120"/>
-      <c r="D201" s="121"/>
+      <c r="C201" s="106"/>
+      <c r="D201" s="107"/>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
@@ -5753,8 +5753,8 @@
       <c r="B202" s="62" t="s">
         <v>198</v>
       </c>
-      <c r="C202" s="120"/>
-      <c r="D202" s="121"/>
+      <c r="C202" s="106"/>
+      <c r="D202" s="107"/>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
@@ -5763,8 +5763,8 @@
       <c r="B203" s="58" t="s">
         <v>199</v>
       </c>
-      <c r="C203" s="134"/>
-      <c r="D203" s="135"/>
+      <c r="C203" s="121"/>
+      <c r="D203" s="122"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
@@ -5773,16 +5773,16 @@
       <c r="B204" s="58" t="s">
         <v>200</v>
       </c>
-      <c r="C204" s="134"/>
-      <c r="D204" s="135"/>
+      <c r="C204" s="121"/>
+      <c r="D204" s="122"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A205" s="1"/>
-      <c r="B205" s="116" t="s">
+      <c r="B205" s="108" t="s">
         <v>201</v>
       </c>
-      <c r="C205" s="117"/>
-      <c r="D205" s="118"/>
+      <c r="C205" s="109"/>
+      <c r="D205" s="110"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
@@ -5791,8 +5791,8 @@
       <c r="B206" s="62" t="s">
         <v>202</v>
       </c>
-      <c r="C206" s="120"/>
-      <c r="D206" s="121"/>
+      <c r="C206" s="106"/>
+      <c r="D206" s="107"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
@@ -5801,8 +5801,8 @@
       <c r="B207" s="13" t="s">
         <v>203</v>
       </c>
-      <c r="C207" s="136"/>
-      <c r="D207" s="123"/>
+      <c r="C207" s="123"/>
+      <c r="D207" s="112"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
@@ -5811,8 +5811,8 @@
       <c r="B208" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="C208" s="122"/>
-      <c r="D208" s="123"/>
+      <c r="C208" s="116"/>
+      <c r="D208" s="112"/>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
@@ -5821,8 +5821,8 @@
       <c r="B209" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="C209" s="122"/>
-      <c r="D209" s="123"/>
+      <c r="C209" s="116"/>
+      <c r="D209" s="112"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
@@ -5831,8 +5831,8 @@
       <c r="B210" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="C210" s="122"/>
-      <c r="D210" s="123"/>
+      <c r="C210" s="116"/>
+      <c r="D210" s="112"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
@@ -5841,16 +5841,16 @@
       <c r="B211" s="13" t="s">
         <v>207</v>
       </c>
-      <c r="C211" s="122"/>
-      <c r="D211" s="123"/>
+      <c r="C211" s="116"/>
+      <c r="D211" s="112"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A212" s="1"/>
-      <c r="B212" s="116" t="s">
+      <c r="B212" s="108" t="s">
         <v>208</v>
       </c>
-      <c r="C212" s="117"/>
-      <c r="D212" s="118"/>
+      <c r="C212" s="109"/>
+      <c r="D212" s="110"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A213" s="1">
@@ -5859,8 +5859,8 @@
       <c r="B213" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="C213" s="120"/>
-      <c r="D213" s="121"/>
+      <c r="C213" s="106"/>
+      <c r="D213" s="107"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A214" s="1">
@@ -5869,8 +5869,8 @@
       <c r="B214" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="C214" s="120"/>
-      <c r="D214" s="121"/>
+      <c r="C214" s="106"/>
+      <c r="D214" s="107"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A215" s="1">
@@ -5879,8 +5879,8 @@
       <c r="B215" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="C215" s="120"/>
-      <c r="D215" s="121"/>
+      <c r="C215" s="106"/>
+      <c r="D215" s="107"/>
     </row>
     <row r="216" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A216" s="26">
@@ -5889,11 +5889,164 @@
       <c r="B216" s="14" t="s">
         <v>212</v>
       </c>
-      <c r="C216" s="132"/>
-      <c r="D216" s="133"/>
+      <c r="C216" s="119"/>
+      <c r="D216" s="120"/>
     </row>
   </sheetData>
   <mergeCells count="177">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A1:D2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="C54:D54"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="C91:D91"/>
+    <mergeCell ref="B48:D48"/>
+    <mergeCell ref="B49:D49"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="C59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="C61:D61"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="C64:D64"/>
+    <mergeCell ref="C65:D65"/>
+    <mergeCell ref="C66:D66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="C68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C70:D70"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="C72:D72"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C76:D76"/>
+    <mergeCell ref="C77:D77"/>
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C79:D79"/>
+    <mergeCell ref="B95:D95"/>
+    <mergeCell ref="C96:D96"/>
+    <mergeCell ref="C92:D92"/>
+    <mergeCell ref="C93:D93"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="C83:D83"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="C103:D103"/>
+    <mergeCell ref="C104:D104"/>
+    <mergeCell ref="C105:D105"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="C107:D107"/>
+    <mergeCell ref="C97:D97"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C99:D99"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="C102:D102"/>
+    <mergeCell ref="C113:D113"/>
+    <mergeCell ref="C114:D114"/>
+    <mergeCell ref="C115:D115"/>
+    <mergeCell ref="C116:D116"/>
+    <mergeCell ref="C117:D117"/>
+    <mergeCell ref="C118:D118"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="C109:D109"/>
+    <mergeCell ref="C110:D110"/>
+    <mergeCell ref="C111:D111"/>
+    <mergeCell ref="C112:D112"/>
+    <mergeCell ref="C125:D125"/>
+    <mergeCell ref="B126:D126"/>
+    <mergeCell ref="C127:D127"/>
+    <mergeCell ref="C128:D128"/>
+    <mergeCell ref="C129:D129"/>
+    <mergeCell ref="C130:D130"/>
+    <mergeCell ref="C119:D119"/>
+    <mergeCell ref="C120:D120"/>
+    <mergeCell ref="C121:D121"/>
+    <mergeCell ref="C122:D122"/>
+    <mergeCell ref="C123:D123"/>
+    <mergeCell ref="C124:D124"/>
+    <mergeCell ref="C137:D137"/>
+    <mergeCell ref="C138:D138"/>
+    <mergeCell ref="C139:D139"/>
+    <mergeCell ref="C140:D140"/>
+    <mergeCell ref="C141:D141"/>
+    <mergeCell ref="C142:D142"/>
+    <mergeCell ref="B131:D131"/>
+    <mergeCell ref="C132:D132"/>
+    <mergeCell ref="C133:D133"/>
+    <mergeCell ref="C134:D134"/>
+    <mergeCell ref="C135:D135"/>
+    <mergeCell ref="C136:D136"/>
+    <mergeCell ref="B150:D150"/>
+    <mergeCell ref="B159:D159"/>
+    <mergeCell ref="C160:D160"/>
+    <mergeCell ref="C161:D161"/>
+    <mergeCell ref="C162:D162"/>
+    <mergeCell ref="C163:D163"/>
+    <mergeCell ref="B144:D144"/>
+    <mergeCell ref="C145:D145"/>
+    <mergeCell ref="B146:D146"/>
+    <mergeCell ref="C147:D147"/>
+    <mergeCell ref="C148:D148"/>
+    <mergeCell ref="C149:D149"/>
+    <mergeCell ref="B183:D183"/>
+    <mergeCell ref="C184:D184"/>
+    <mergeCell ref="B176:D176"/>
+    <mergeCell ref="C177:D177"/>
+    <mergeCell ref="C178:D178"/>
+    <mergeCell ref="C164:D164"/>
+    <mergeCell ref="C165:D165"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="C167:D167"/>
+    <mergeCell ref="C215:D215"/>
+    <mergeCell ref="C216:D216"/>
+    <mergeCell ref="C209:D209"/>
+    <mergeCell ref="C210:D210"/>
+    <mergeCell ref="C211:D211"/>
+    <mergeCell ref="B212:D212"/>
+    <mergeCell ref="C213:D213"/>
+    <mergeCell ref="C203:D203"/>
+    <mergeCell ref="C204:D204"/>
+    <mergeCell ref="B205:D205"/>
+    <mergeCell ref="C206:D206"/>
+    <mergeCell ref="C207:D207"/>
+    <mergeCell ref="C208:D208"/>
     <mergeCell ref="C197:D197"/>
     <mergeCell ref="C198:D198"/>
     <mergeCell ref="B199:D199"/>
@@ -5918,159 +6071,6 @@
     <mergeCell ref="B180:D180"/>
     <mergeCell ref="C181:D181"/>
     <mergeCell ref="C182:D182"/>
-    <mergeCell ref="C215:D215"/>
-    <mergeCell ref="C216:D216"/>
-    <mergeCell ref="C209:D209"/>
-    <mergeCell ref="C210:D210"/>
-    <mergeCell ref="C211:D211"/>
-    <mergeCell ref="B212:D212"/>
-    <mergeCell ref="C213:D213"/>
-    <mergeCell ref="C203:D203"/>
-    <mergeCell ref="C204:D204"/>
-    <mergeCell ref="B205:D205"/>
-    <mergeCell ref="C206:D206"/>
-    <mergeCell ref="C207:D207"/>
-    <mergeCell ref="C208:D208"/>
-    <mergeCell ref="B183:D183"/>
-    <mergeCell ref="C184:D184"/>
-    <mergeCell ref="B176:D176"/>
-    <mergeCell ref="C177:D177"/>
-    <mergeCell ref="C178:D178"/>
-    <mergeCell ref="C164:D164"/>
-    <mergeCell ref="C165:D165"/>
-    <mergeCell ref="C166:D166"/>
-    <mergeCell ref="C167:D167"/>
-    <mergeCell ref="B150:D150"/>
-    <mergeCell ref="B159:D159"/>
-    <mergeCell ref="C160:D160"/>
-    <mergeCell ref="C161:D161"/>
-    <mergeCell ref="C162:D162"/>
-    <mergeCell ref="C163:D163"/>
-    <mergeCell ref="B144:D144"/>
-    <mergeCell ref="C145:D145"/>
-    <mergeCell ref="B146:D146"/>
-    <mergeCell ref="C147:D147"/>
-    <mergeCell ref="C148:D148"/>
-    <mergeCell ref="C149:D149"/>
-    <mergeCell ref="C137:D137"/>
-    <mergeCell ref="C138:D138"/>
-    <mergeCell ref="C139:D139"/>
-    <mergeCell ref="C140:D140"/>
-    <mergeCell ref="C141:D141"/>
-    <mergeCell ref="C142:D142"/>
-    <mergeCell ref="B131:D131"/>
-    <mergeCell ref="C132:D132"/>
-    <mergeCell ref="C133:D133"/>
-    <mergeCell ref="C134:D134"/>
-    <mergeCell ref="C135:D135"/>
-    <mergeCell ref="C136:D136"/>
-    <mergeCell ref="C125:D125"/>
-    <mergeCell ref="B126:D126"/>
-    <mergeCell ref="C127:D127"/>
-    <mergeCell ref="C128:D128"/>
-    <mergeCell ref="C129:D129"/>
-    <mergeCell ref="C130:D130"/>
-    <mergeCell ref="C119:D119"/>
-    <mergeCell ref="C120:D120"/>
-    <mergeCell ref="C121:D121"/>
-    <mergeCell ref="C122:D122"/>
-    <mergeCell ref="C123:D123"/>
-    <mergeCell ref="C124:D124"/>
-    <mergeCell ref="C113:D113"/>
-    <mergeCell ref="C114:D114"/>
-    <mergeCell ref="C115:D115"/>
-    <mergeCell ref="C116:D116"/>
-    <mergeCell ref="C117:D117"/>
-    <mergeCell ref="C118:D118"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C112:D112"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="B106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="B95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="B48:D48"/>
-    <mergeCell ref="B49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="B58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A1:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="68" fitToHeight="100" orientation="portrait" r:id="rId1"/>
@@ -6119,10 +6119,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="128" t="s">
         <v>214</v>
       </c>
-      <c r="C4" s="125"/>
+      <c r="C4" s="129"/>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="50">
@@ -6198,10 +6198,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="51"/>
-      <c r="B13" s="124" t="s">
+      <c r="B13" s="128" t="s">
         <v>223</v>
       </c>
-      <c r="C13" s="125"/>
+      <c r="C13" s="129"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
@@ -6266,7 +6266,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="12"/>
-      <c r="B21" s="124" t="s">
+      <c r="B21" s="128" t="s">
         <v>225</v>
       </c>
       <c r="C21" s="143"/>
@@ -6548,10 +6548,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="12"/>
-      <c r="B53" s="124" t="s">
+      <c r="B53" s="128" t="s">
         <v>256</v>
       </c>
-      <c r="C53" s="125"/>
+      <c r="C53" s="129"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="12">
@@ -6642,10 +6642,10 @@
     </row>
     <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="15"/>
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="128" t="s">
         <v>214</v>
       </c>
-      <c r="C4" s="125"/>
+      <c r="C4" s="129"/>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="50">
@@ -6721,10 +6721,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="51"/>
-      <c r="B13" s="124" t="s">
+      <c r="B13" s="128" t="s">
         <v>223</v>
       </c>
-      <c r="C13" s="125"/>
+      <c r="C13" s="129"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="12">
@@ -6789,7 +6789,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="12"/>
-      <c r="B21" s="124" t="s">
+      <c r="B21" s="128" t="s">
         <v>225</v>
       </c>
       <c r="C21" s="143"/>
@@ -7055,10 +7055,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="12"/>
-      <c r="B51" s="124" t="s">
+      <c r="B51" s="128" t="s">
         <v>256</v>
       </c>
-      <c r="C51" s="125"/>
+      <c r="C51" s="129"/>
     </row>
     <row r="52" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="12">
@@ -7112,7 +7112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C195"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A180" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A180" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="90" workbookViewId="0">
       <selection activeCell="F195" sqref="F195"/>
     </sheetView>
   </sheetViews>
@@ -7145,10 +7145,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="51"/>
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="128" t="s">
         <v>214</v>
       </c>
-      <c r="C4" s="125"/>
+      <c r="C4" s="129"/>
     </row>
     <row r="5" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="50">
@@ -7227,7 +7227,7 @@
       <c r="B13" s="150" t="s">
         <v>224</v>
       </c>
-      <c r="C13" s="156"/>
+      <c r="C13" s="161"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="50">
@@ -7258,10 +7258,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="51"/>
-      <c r="B17" s="124" t="s">
+      <c r="B17" s="128" t="s">
         <v>223</v>
       </c>
-      <c r="C17" s="125"/>
+      <c r="C17" s="129"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="12">
@@ -7292,7 +7292,7 @@
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="12"/>
-      <c r="B21" s="124" t="s">
+      <c r="B21" s="128" t="s">
         <v>225</v>
       </c>
       <c r="C21" s="143"/>
@@ -7574,10 +7574,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="12"/>
-      <c r="B53" s="124" t="s">
+      <c r="B53" s="128" t="s">
         <v>256</v>
       </c>
-      <c r="C53" s="125"/>
+      <c r="C53" s="129"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="12">
@@ -7771,10 +7771,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="54"/>
-      <c r="B76" s="157" t="s">
+      <c r="B76" s="152" t="s">
         <v>280</v>
       </c>
-      <c r="C76" s="158"/>
+      <c r="C76" s="153"/>
     </row>
     <row r="77" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="55">
@@ -7841,10 +7841,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A84" s="54"/>
-      <c r="B84" s="157" t="s">
+      <c r="B84" s="152" t="s">
         <v>288</v>
       </c>
-      <c r="C84" s="158"/>
+      <c r="C84" s="153"/>
     </row>
     <row r="85" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="55">
@@ -7918,10 +7918,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A93" s="54"/>
-      <c r="B93" s="157" t="s">
+      <c r="B93" s="152" t="s">
         <v>297</v>
       </c>
-      <c r="C93" s="158"/>
+      <c r="C93" s="153"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A94" s="55">
@@ -7979,10 +7979,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A100" s="54"/>
-      <c r="B100" s="157" t="s">
+      <c r="B100" s="152" t="s">
         <v>304</v>
       </c>
-      <c r="C100" s="158"/>
+      <c r="C100" s="153"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A101" s="55">
@@ -8022,10 +8022,10 @@
     </row>
     <row r="105" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="55"/>
-      <c r="B105" s="152" t="s">
+      <c r="B105" s="154" t="s">
         <v>306</v>
       </c>
-      <c r="C105" s="159"/>
+      <c r="C105" s="158"/>
     </row>
     <row r="106" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="55">
@@ -8056,10 +8056,10 @@
     </row>
     <row r="109" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="54"/>
-      <c r="B109" s="157" t="s">
+      <c r="B109" s="152" t="s">
         <v>309</v>
       </c>
-      <c r="C109" s="158"/>
+      <c r="C109" s="153"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A110" s="55">
@@ -8117,10 +8117,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A116" s="54"/>
-      <c r="B116" s="157" t="s">
+      <c r="B116" s="152" t="s">
         <v>311</v>
       </c>
-      <c r="C116" s="158"/>
+      <c r="C116" s="153"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A117" s="55">
@@ -8178,10 +8178,10 @@
     </row>
     <row r="123" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="54"/>
-      <c r="B123" s="157" t="s">
+      <c r="B123" s="152" t="s">
         <v>313</v>
       </c>
-      <c r="C123" s="158"/>
+      <c r="C123" s="153"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A124" s="55">
@@ -8239,10 +8239,10 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A130" s="54"/>
-      <c r="B130" s="157" t="s">
+      <c r="B130" s="152" t="s">
         <v>314</v>
       </c>
-      <c r="C130" s="158"/>
+      <c r="C130" s="153"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A131" s="55">
@@ -8300,10 +8300,10 @@
     </row>
     <row r="137" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" s="54"/>
-      <c r="B137" s="157" t="s">
+      <c r="B137" s="152" t="s">
         <v>315</v>
       </c>
-      <c r="C137" s="158"/>
+      <c r="C137" s="153"/>
     </row>
     <row r="138" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" s="55">
@@ -8361,10 +8361,10 @@
     </row>
     <row r="144" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" s="55"/>
-      <c r="B144" s="152" t="s">
+      <c r="B144" s="154" t="s">
         <v>134</v>
       </c>
-      <c r="C144" s="153"/>
+      <c r="C144" s="155"/>
     </row>
     <row r="145" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" s="55">
@@ -8422,10 +8422,10 @@
     </row>
     <row r="151" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" s="55"/>
-      <c r="B151" s="154" t="s">
+      <c r="B151" s="159" t="s">
         <v>322</v>
       </c>
-      <c r="C151" s="155"/>
+      <c r="C151" s="160"/>
     </row>
     <row r="152" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" s="55">
@@ -8483,10 +8483,10 @@
     </row>
     <row r="158" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" s="54"/>
-      <c r="B158" s="157" t="s">
+      <c r="B158" s="152" t="s">
         <v>329</v>
       </c>
-      <c r="C158" s="158"/>
+      <c r="C158" s="153"/>
     </row>
     <row r="159" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" s="55">
@@ -8517,10 +8517,10 @@
     </row>
     <row r="162" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="54"/>
-      <c r="B162" s="157" t="s">
+      <c r="B162" s="152" t="s">
         <v>333</v>
       </c>
-      <c r="C162" s="158"/>
+      <c r="C162" s="153"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A163" s="55">
@@ -8551,10 +8551,10 @@
     </row>
     <row r="166" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="54"/>
-      <c r="B166" s="157" t="s">
+      <c r="B166" s="152" t="s">
         <v>337</v>
       </c>
-      <c r="C166" s="158"/>
+      <c r="C166" s="153"/>
     </row>
     <row r="167" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="55">
@@ -8675,10 +8675,10 @@
     </row>
     <row r="180" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="55"/>
-      <c r="B180" s="152" t="s">
+      <c r="B180" s="154" t="s">
         <v>351</v>
       </c>
-      <c r="C180" s="153"/>
+      <c r="C180" s="155"/>
     </row>
     <row r="181" spans="1:3" ht="26" x14ac:dyDescent="0.35">
       <c r="A181" s="55">
@@ -8772,10 +8772,10 @@
     </row>
     <row r="191" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" s="56"/>
-      <c r="B191" s="160" t="s">
+      <c r="B191" s="156" t="s">
         <v>362</v>
       </c>
-      <c r="C191" s="161"/>
+      <c r="C191" s="157"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A192" s="55">
@@ -8815,21 +8815,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B158:C158"/>
-    <mergeCell ref="B162:C162"/>
-    <mergeCell ref="B166:C166"/>
-    <mergeCell ref="B180:C180"/>
-    <mergeCell ref="B191:C191"/>
-    <mergeCell ref="B105:C105"/>
-    <mergeCell ref="B109:C109"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B130:C130"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B93:C93"/>
-    <mergeCell ref="B100:C100"/>
     <mergeCell ref="B144:C144"/>
     <mergeCell ref="B151:C151"/>
     <mergeCell ref="B61:C61"/>
@@ -8846,6 +8831,21 @@
     <mergeCell ref="B57:C57"/>
     <mergeCell ref="B137:C137"/>
     <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B93:C93"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B130:C130"/>
+    <mergeCell ref="B158:C158"/>
+    <mergeCell ref="B162:C162"/>
+    <mergeCell ref="B166:C166"/>
+    <mergeCell ref="B180:C180"/>
+    <mergeCell ref="B191:C191"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="87" fitToHeight="100" orientation="portrait" r:id="rId1"/>

</xml_diff>